<commit_message>
multi clients handler added
</commit_message>
<xml_diff>
--- a/mcd.xlsx
+++ b/mcd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamilgolawski/Nauka/Programowanie/Python/autoOdbiory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCBDEC7-6F08-3544-88DB-D40D649BCF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC0DA6B-E50A-694C-A071-5D6AE8E916C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{E828F9E1-35FF-9446-80FB-16E4BC99432C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Adres</t>
   </si>
@@ -63,6 +63,27 @@
   </si>
   <si>
     <t>Aleja Spółdzielczości Pracy 34, 20-147 Lublin</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>Priorytety</t>
+  </si>
+  <si>
+    <t>al. Wincentego Witosa 32, 20-315 Lublin</t>
+  </si>
+  <si>
+    <t>al. Tysiąclecia 12, 20-121 Lublin</t>
+  </si>
+  <si>
+    <t>Ireny Sendlerowej 1, 20-817 Lublin</t>
+  </si>
+  <si>
+    <t>KFC</t>
   </si>
 </sst>
 </file>
@@ -434,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A21D65C-CA10-484E-9F2F-28C9D9AD30E3}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,49 +466,136 @@
     <col min="1" max="1" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>